<commit_message>
Adding a stat distribution tester to ensure formulas will work
</commit_message>
<xml_diff>
--- a/SEPARATE - Combat Simulator/classFinalStats.xlsx
+++ b/SEPARATE - Combat Simulator/classFinalStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\Projects\FlaskSimpleRPG\SEPARATE - Combat Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4526732-50A4-4C9D-982D-BF8A79C24571}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02C2291-23BA-4C4E-9F7F-AAC69134B657}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10CED9EE-287C-4692-89A8-1ACF3A1E842F}"/>
   </bookViews>
@@ -676,8 +676,8 @@
   <dimension ref="A1:R181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K111" sqref="K111"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +795,7 @@
         <v>350010</v>
       </c>
       <c r="N2" s="1">
-        <v>7080060</v>
+        <v>8260060</v>
       </c>
       <c r="O2">
         <v>1050</v>
@@ -851,7 +851,7 @@
         <v>357010</v>
       </c>
       <c r="N3" s="1">
-        <v>7200060</v>
+        <v>8400060</v>
       </c>
       <c r="O3">
         <v>1071</v>
@@ -907,7 +907,7 @@
         <v>367510</v>
       </c>
       <c r="N4" s="1">
-        <v>7440060</v>
+        <v>8680060</v>
       </c>
       <c r="O4">
         <v>1102</v>
@@ -963,7 +963,7 @@
         <v>381510</v>
       </c>
       <c r="N5" s="1">
-        <v>7680060</v>
+        <v>8960060</v>
       </c>
       <c r="O5">
         <v>1144</v>
@@ -1019,7 +1019,7 @@
         <v>402510</v>
       </c>
       <c r="N6" s="1">
-        <v>8160060</v>
+        <v>9520060</v>
       </c>
       <c r="O6">
         <v>1207</v>
@@ -1075,7 +1075,7 @@
         <v>333343</v>
       </c>
       <c r="N7" s="1">
-        <v>6720060</v>
+        <v>7840060</v>
       </c>
       <c r="O7">
         <v>1000</v>
@@ -1131,7 +1131,7 @@
         <v>340010</v>
       </c>
       <c r="N8" s="1">
-        <v>6840060</v>
+        <v>7980060</v>
       </c>
       <c r="O8">
         <v>1020</v>
@@ -1187,7 +1187,7 @@
         <v>350010</v>
       </c>
       <c r="N9" s="1">
-        <v>7080060</v>
+        <v>8260060</v>
       </c>
       <c r="O9">
         <v>1050</v>
@@ -1243,7 +1243,7 @@
         <v>363343</v>
       </c>
       <c r="N10" s="1">
-        <v>7320060</v>
+        <v>8540060</v>
       </c>
       <c r="O10">
         <v>1090</v>
@@ -1299,7 +1299,7 @@
         <v>383343</v>
       </c>
       <c r="N11" s="1">
-        <v>7800060</v>
+        <v>9100060</v>
       </c>
       <c r="O11">
         <v>1150</v>
@@ -1355,7 +1355,7 @@
         <v>316676</v>
       </c>
       <c r="N12" s="1">
-        <v>6360060</v>
+        <v>7420060</v>
       </c>
       <c r="O12">
         <v>950</v>
@@ -1411,7 +1411,7 @@
         <v>323010</v>
       </c>
       <c r="N13" s="1">
-        <v>6480060</v>
+        <v>7560060</v>
       </c>
       <c r="O13">
         <v>969</v>
@@ -1467,7 +1467,7 @@
         <v>332510</v>
       </c>
       <c r="N14" s="1">
-        <v>6720060</v>
+        <v>7840060</v>
       </c>
       <c r="O14">
         <v>997</v>
@@ -1523,7 +1523,7 @@
         <v>345176</v>
       </c>
       <c r="N15" s="1">
-        <v>6960060</v>
+        <v>8120060</v>
       </c>
       <c r="O15">
         <v>1035</v>
@@ -1570,7 +1570,7 @@
         <v>3104</v>
       </c>
       <c r="K16">
-        <v>50</v>
+        <v>51.7</v>
       </c>
       <c r="L16">
         <v>23.7</v>
@@ -1579,7 +1579,7 @@
         <v>364176</v>
       </c>
       <c r="N16" s="1">
-        <v>7320060</v>
+        <v>8540060</v>
       </c>
       <c r="O16">
         <v>1092</v>
@@ -1635,7 +1635,7 @@
         <v>350010</v>
       </c>
       <c r="N17" s="1">
-        <v>5900060</v>
+        <v>6608060</v>
       </c>
       <c r="O17">
         <v>1050</v>
@@ -1691,7 +1691,7 @@
         <v>357010</v>
       </c>
       <c r="N18" s="1">
-        <v>6000060</v>
+        <v>6720060</v>
       </c>
       <c r="O18">
         <v>1071</v>
@@ -1747,7 +1747,7 @@
         <v>367510</v>
       </c>
       <c r="N19" s="1">
-        <v>6200060</v>
+        <v>6944060</v>
       </c>
       <c r="O19">
         <v>1102</v>
@@ -1803,7 +1803,7 @@
         <v>381510</v>
       </c>
       <c r="N20" s="1">
-        <v>6400060</v>
+        <v>7168060</v>
       </c>
       <c r="O20">
         <v>1144</v>
@@ -1859,7 +1859,7 @@
         <v>402510</v>
       </c>
       <c r="N21" s="1">
-        <v>6800060</v>
+        <v>7616060</v>
       </c>
       <c r="O21">
         <v>1207</v>
@@ -1915,7 +1915,7 @@
         <v>333343</v>
       </c>
       <c r="N22" s="1">
-        <v>5600060</v>
+        <v>6272060</v>
       </c>
       <c r="O22">
         <v>1000</v>
@@ -1971,7 +1971,7 @@
         <v>340010</v>
       </c>
       <c r="N23" s="1">
-        <v>5700060</v>
+        <v>6384060</v>
       </c>
       <c r="O23">
         <v>1020</v>
@@ -2027,7 +2027,7 @@
         <v>350010</v>
       </c>
       <c r="N24" s="1">
-        <v>5900060</v>
+        <v>6608060</v>
       </c>
       <c r="O24">
         <v>1050</v>
@@ -2083,7 +2083,7 @@
         <v>363343</v>
       </c>
       <c r="N25" s="1">
-        <v>6100060</v>
+        <v>6832060</v>
       </c>
       <c r="O25">
         <v>1090</v>
@@ -2139,7 +2139,7 @@
         <v>383343</v>
       </c>
       <c r="N26" s="1">
-        <v>6500060</v>
+        <v>7280060</v>
       </c>
       <c r="O26">
         <v>1150</v>
@@ -2186,7 +2186,7 @@
         <v>2700</v>
       </c>
       <c r="K27">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="L27">
         <v>20.6</v>
@@ -2195,7 +2195,7 @@
         <v>316676</v>
       </c>
       <c r="N27" s="1">
-        <v>5300060</v>
+        <v>5936060</v>
       </c>
       <c r="O27">
         <v>950</v>
@@ -2242,7 +2242,7 @@
         <v>2754</v>
       </c>
       <c r="K28">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="L28">
         <v>21</v>
@@ -2251,7 +2251,7 @@
         <v>323010</v>
       </c>
       <c r="N28" s="1">
-        <v>5400060</v>
+        <v>6048060</v>
       </c>
       <c r="O28">
         <v>969</v>
@@ -2298,7 +2298,7 @@
         <v>2835</v>
       </c>
       <c r="K29">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="L29">
         <v>21.6</v>
@@ -2307,7 +2307,7 @@
         <v>332510</v>
       </c>
       <c r="N29" s="1">
-        <v>5600060</v>
+        <v>6272060</v>
       </c>
       <c r="O29">
         <v>997</v>
@@ -2354,7 +2354,7 @@
         <v>2943</v>
       </c>
       <c r="K30">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="L30">
         <v>22.4</v>
@@ -2363,7 +2363,7 @@
         <v>345176</v>
       </c>
       <c r="N30" s="1">
-        <v>5800060</v>
+        <v>6496060</v>
       </c>
       <c r="O30">
         <v>1035</v>
@@ -2410,7 +2410,7 @@
         <v>3104</v>
       </c>
       <c r="K31">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="L31">
         <v>23.7</v>
@@ -2419,7 +2419,7 @@
         <v>364176</v>
       </c>
       <c r="N31" s="1">
-        <v>6100060</v>
+        <v>6832060</v>
       </c>
       <c r="O31">
         <v>1092</v>
@@ -2475,7 +2475,7 @@
         <v>350010</v>
       </c>
       <c r="N32" s="1">
-        <v>6608060</v>
+        <v>7080060</v>
       </c>
       <c r="O32">
         <v>1050</v>
@@ -2531,7 +2531,7 @@
         <v>357010</v>
       </c>
       <c r="N33" s="1">
-        <v>6720060</v>
+        <v>7200060</v>
       </c>
       <c r="O33">
         <v>1071</v>
@@ -2587,7 +2587,7 @@
         <v>367510</v>
       </c>
       <c r="N34" s="1">
-        <v>6944060</v>
+        <v>7440060</v>
       </c>
       <c r="O34">
         <v>1102</v>
@@ -2643,7 +2643,7 @@
         <v>381510</v>
       </c>
       <c r="N35" s="1">
-        <v>7168060</v>
+        <v>7680060</v>
       </c>
       <c r="O35">
         <v>1144</v>
@@ -2699,7 +2699,7 @@
         <v>402510</v>
       </c>
       <c r="N36" s="1">
-        <v>7616060</v>
+        <v>8160060</v>
       </c>
       <c r="O36">
         <v>1207</v>
@@ -2755,7 +2755,7 @@
         <v>333343</v>
       </c>
       <c r="N37" s="1">
-        <v>6272060</v>
+        <v>6720060</v>
       </c>
       <c r="O37">
         <v>1000</v>
@@ -2811,7 +2811,7 @@
         <v>340010</v>
       </c>
       <c r="N38" s="1">
-        <v>6384060</v>
+        <v>6840060</v>
       </c>
       <c r="O38">
         <v>1020</v>
@@ -2867,7 +2867,7 @@
         <v>350010</v>
       </c>
       <c r="N39" s="1">
-        <v>6608060</v>
+        <v>7080060</v>
       </c>
       <c r="O39">
         <v>1050</v>
@@ -2923,7 +2923,7 @@
         <v>363343</v>
       </c>
       <c r="N40" s="1">
-        <v>6832060</v>
+        <v>7320060</v>
       </c>
       <c r="O40">
         <v>1090</v>
@@ -2979,7 +2979,7 @@
         <v>383343</v>
       </c>
       <c r="N41" s="1">
-        <v>7280060</v>
+        <v>7800060</v>
       </c>
       <c r="O41">
         <v>1150</v>
@@ -3035,7 +3035,7 @@
         <v>316676</v>
       </c>
       <c r="N42" s="1">
-        <v>5936060</v>
+        <v>6360060</v>
       </c>
       <c r="O42">
         <v>950</v>
@@ -3082,7 +3082,7 @@
         <v>2754</v>
       </c>
       <c r="K43">
-        <v>45</v>
+        <v>45.9</v>
       </c>
       <c r="L43">
         <v>21</v>
@@ -3091,7 +3091,7 @@
         <v>323010</v>
       </c>
       <c r="N43" s="1">
-        <v>6048060</v>
+        <v>6480060</v>
       </c>
       <c r="O43">
         <v>969</v>
@@ -3138,7 +3138,7 @@
         <v>2835</v>
       </c>
       <c r="K44">
-        <v>45</v>
+        <v>47.3</v>
       </c>
       <c r="L44">
         <v>21.6</v>
@@ -3147,7 +3147,7 @@
         <v>332510</v>
       </c>
       <c r="N44" s="1">
-        <v>6272060</v>
+        <v>6720060</v>
       </c>
       <c r="O44">
         <v>997</v>
@@ -3194,7 +3194,7 @@
         <v>2943</v>
       </c>
       <c r="K45">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="L45">
         <v>22.4</v>
@@ -3203,7 +3203,7 @@
         <v>345176</v>
       </c>
       <c r="N45" s="1">
-        <v>6496060</v>
+        <v>6960060</v>
       </c>
       <c r="O45">
         <v>1035</v>
@@ -3250,7 +3250,7 @@
         <v>3104</v>
       </c>
       <c r="K46">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="L46">
         <v>23.7</v>
@@ -3259,7 +3259,7 @@
         <v>364176</v>
       </c>
       <c r="N46" s="1">
-        <v>6832060</v>
+        <v>7320060</v>
       </c>
       <c r="O46">
         <v>1092</v>
@@ -3315,7 +3315,7 @@
         <v>350010</v>
       </c>
       <c r="N47" s="1">
-        <v>5664060</v>
+        <v>6372060</v>
       </c>
       <c r="O47">
         <v>1050</v>
@@ -3371,7 +3371,7 @@
         <v>357010</v>
       </c>
       <c r="N48" s="1">
-        <v>5760060</v>
+        <v>6480060</v>
       </c>
       <c r="O48">
         <v>1071</v>
@@ -3427,7 +3427,7 @@
         <v>367510</v>
       </c>
       <c r="N49" s="1">
-        <v>5952060</v>
+        <v>6696060</v>
       </c>
       <c r="O49">
         <v>1102</v>
@@ -3483,7 +3483,7 @@
         <v>381510</v>
       </c>
       <c r="N50" s="1">
-        <v>6144060</v>
+        <v>6912060</v>
       </c>
       <c r="O50">
         <v>1144</v>
@@ -3539,7 +3539,7 @@
         <v>402510</v>
       </c>
       <c r="N51" s="1">
-        <v>6528060</v>
+        <v>7344060</v>
       </c>
       <c r="O51">
         <v>1207</v>
@@ -3595,7 +3595,7 @@
         <v>333343</v>
       </c>
       <c r="N52" s="1">
-        <v>5376060</v>
+        <v>6048060</v>
       </c>
       <c r="O52">
         <v>1000</v>
@@ -3651,7 +3651,7 @@
         <v>340010</v>
       </c>
       <c r="N53" s="1">
-        <v>5472060</v>
+        <v>6156060</v>
       </c>
       <c r="O53">
         <v>1020</v>
@@ -3707,7 +3707,7 @@
         <v>350010</v>
       </c>
       <c r="N54" s="1">
-        <v>5664060</v>
+        <v>6372060</v>
       </c>
       <c r="O54">
         <v>1050</v>
@@ -3763,7 +3763,7 @@
         <v>363343</v>
       </c>
       <c r="N55" s="1">
-        <v>5856060</v>
+        <v>6588060</v>
       </c>
       <c r="O55">
         <v>1090</v>
@@ -3819,7 +3819,7 @@
         <v>383343</v>
       </c>
       <c r="N56" s="1">
-        <v>6240060</v>
+        <v>7020060</v>
       </c>
       <c r="O56">
         <v>1150</v>
@@ -3866,7 +3866,7 @@
         <v>2700</v>
       </c>
       <c r="K57">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="L57">
         <v>45.6</v>
@@ -3875,7 +3875,7 @@
         <v>316676</v>
       </c>
       <c r="N57" s="1">
-        <v>5088060</v>
+        <v>5724060</v>
       </c>
       <c r="O57">
         <v>950</v>
@@ -3922,7 +3922,7 @@
         <v>2754</v>
       </c>
       <c r="K58">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="L58">
         <v>46</v>
@@ -3931,7 +3931,7 @@
         <v>323010</v>
       </c>
       <c r="N58" s="1">
-        <v>5184060</v>
+        <v>5832060</v>
       </c>
       <c r="O58">
         <v>969</v>
@@ -3978,7 +3978,7 @@
         <v>2835</v>
       </c>
       <c r="K59">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="L59">
         <v>46.6</v>
@@ -3987,7 +3987,7 @@
         <v>332510</v>
       </c>
       <c r="N59" s="1">
-        <v>5376060</v>
+        <v>6048060</v>
       </c>
       <c r="O59">
         <v>997</v>
@@ -4034,7 +4034,7 @@
         <v>2943</v>
       </c>
       <c r="K60">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="L60">
         <v>47.4</v>
@@ -4043,7 +4043,7 @@
         <v>345176</v>
       </c>
       <c r="N60" s="1">
-        <v>5568060</v>
+        <v>6264060</v>
       </c>
       <c r="O60">
         <v>1035</v>
@@ -4090,7 +4090,7 @@
         <v>3104</v>
       </c>
       <c r="K61">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="L61">
         <v>48.7</v>
@@ -4099,7 +4099,7 @@
         <v>364176</v>
       </c>
       <c r="N61" s="1">
-        <v>5856060</v>
+        <v>6588060</v>
       </c>
       <c r="O61">
         <v>1092</v>
@@ -4155,7 +4155,7 @@
         <v>840012</v>
       </c>
       <c r="N62" s="1">
-        <v>4992060</v>
+        <v>4784060</v>
       </c>
       <c r="O62">
         <v>262</v>
@@ -4211,7 +4211,7 @@
         <v>856812</v>
       </c>
       <c r="N63" s="1">
-        <v>5088060</v>
+        <v>4876060</v>
       </c>
       <c r="O63">
         <v>267</v>
@@ -4267,7 +4267,7 @@
         <v>882012</v>
       </c>
       <c r="N64" s="1">
-        <v>5280060</v>
+        <v>5060060</v>
       </c>
       <c r="O64">
         <v>275</v>
@@ -4323,7 +4323,7 @@
         <v>915612</v>
       </c>
       <c r="N65" s="1">
-        <v>5472060</v>
+        <v>5244060</v>
       </c>
       <c r="O65">
         <v>286</v>
@@ -4379,7 +4379,7 @@
         <v>966012</v>
       </c>
       <c r="N66" s="1">
-        <v>5760060</v>
+        <v>5520060</v>
       </c>
       <c r="O66">
         <v>301</v>
@@ -4435,7 +4435,7 @@
         <v>800011.2</v>
       </c>
       <c r="N67" s="1">
-        <v>4800060</v>
+        <v>4600060</v>
       </c>
       <c r="O67">
         <v>250</v>
@@ -4491,7 +4491,7 @@
         <v>816012</v>
       </c>
       <c r="N68" s="1">
-        <v>4896060</v>
+        <v>4692060</v>
       </c>
       <c r="O68">
         <v>255</v>
@@ -4547,7 +4547,7 @@
         <v>840012</v>
       </c>
       <c r="N69" s="1">
-        <v>4992060</v>
+        <v>4784060</v>
       </c>
       <c r="O69">
         <v>262</v>
@@ -4603,7 +4603,7 @@
         <v>872011.2</v>
       </c>
       <c r="N70" s="1">
-        <v>5184060</v>
+        <v>4968060</v>
       </c>
       <c r="O70">
         <v>272</v>
@@ -4659,7 +4659,7 @@
         <v>920011.2</v>
       </c>
       <c r="N71" s="1">
-        <v>5472060</v>
+        <v>5244060</v>
       </c>
       <c r="O71">
         <v>287</v>
@@ -4715,7 +4715,7 @@
         <v>760011.6</v>
       </c>
       <c r="N72" s="1">
-        <v>4512060</v>
+        <v>4324060</v>
       </c>
       <c r="O72">
         <v>237</v>
@@ -4771,7 +4771,7 @@
         <v>775212</v>
       </c>
       <c r="N73" s="1">
-        <v>4608060</v>
+        <v>4416060</v>
       </c>
       <c r="O73">
         <v>242</v>
@@ -4827,7 +4827,7 @@
         <v>798012</v>
       </c>
       <c r="N74" s="1">
-        <v>4704060</v>
+        <v>4508060</v>
       </c>
       <c r="O74">
         <v>249</v>
@@ -4883,7 +4883,7 @@
         <v>828411.6</v>
       </c>
       <c r="N75" s="1">
-        <v>4896060</v>
+        <v>4692060</v>
       </c>
       <c r="O75">
         <v>258</v>
@@ -4939,7 +4939,7 @@
         <v>874011.6</v>
       </c>
       <c r="N76" s="1">
-        <v>5184060</v>
+        <v>4968060</v>
       </c>
       <c r="O76">
         <v>273</v>
@@ -4992,10 +4992,10 @@
         <v>26.3</v>
       </c>
       <c r="M77" s="1">
-        <v>882012</v>
+        <v>252012</v>
       </c>
       <c r="N77" s="1">
-        <v>4368060</v>
+        <v>3744060</v>
       </c>
       <c r="O77">
         <v>262</v>
@@ -5048,10 +5048,10 @@
         <v>26.8</v>
       </c>
       <c r="M78" s="1">
-        <v>899652</v>
+        <v>257052</v>
       </c>
       <c r="N78" s="1">
-        <v>4452060</v>
+        <v>3816060</v>
       </c>
       <c r="O78">
         <v>267</v>
@@ -5104,10 +5104,10 @@
         <v>27.6</v>
       </c>
       <c r="M79" s="1">
-        <v>926112</v>
+        <v>264612</v>
       </c>
       <c r="N79" s="1">
-        <v>4620060</v>
+        <v>3960060</v>
       </c>
       <c r="O79">
         <v>275</v>
@@ -5160,10 +5160,10 @@
         <v>28.6</v>
       </c>
       <c r="M80" s="1">
-        <v>961392</v>
+        <v>274692</v>
       </c>
       <c r="N80" s="1">
-        <v>4788060</v>
+        <v>4104060</v>
       </c>
       <c r="O80">
         <v>286</v>
@@ -5216,10 +5216,10 @@
         <v>30</v>
       </c>
       <c r="M81" s="1">
-        <v>1014312</v>
+        <v>289812</v>
       </c>
       <c r="N81" s="1">
-        <v>5040060</v>
+        <v>4320060</v>
       </c>
       <c r="O81">
         <v>301</v>
@@ -5266,16 +5266,16 @@
         <v>1500</v>
       </c>
       <c r="K82">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L82">
         <v>25</v>
       </c>
       <c r="M82" s="1">
-        <v>840012</v>
+        <v>240012</v>
       </c>
       <c r="N82" s="1">
-        <v>4200060</v>
+        <v>3600060</v>
       </c>
       <c r="O82">
         <v>250</v>
@@ -5322,16 +5322,16 @@
         <v>1530</v>
       </c>
       <c r="K83">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L83">
         <v>25.5</v>
       </c>
       <c r="M83" s="1">
-        <v>856812</v>
+        <v>244812</v>
       </c>
       <c r="N83" s="1">
-        <v>4284060</v>
+        <v>3672060</v>
       </c>
       <c r="O83">
         <v>255</v>
@@ -5378,16 +5378,16 @@
         <v>1575</v>
       </c>
       <c r="K84">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L84">
         <v>26.3</v>
       </c>
       <c r="M84" s="1">
-        <v>882012</v>
+        <v>252012</v>
       </c>
       <c r="N84" s="1">
-        <v>4368060</v>
+        <v>3744060</v>
       </c>
       <c r="O84">
         <v>262</v>
@@ -5434,16 +5434,16 @@
         <v>1635</v>
       </c>
       <c r="K85">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L85">
         <v>27.3</v>
       </c>
       <c r="M85" s="1">
-        <v>915612</v>
+        <v>261612</v>
       </c>
       <c r="N85" s="1">
-        <v>4536060</v>
+        <v>3888060</v>
       </c>
       <c r="O85">
         <v>272</v>
@@ -5490,16 +5490,16 @@
         <v>1724</v>
       </c>
       <c r="K86">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L86">
         <v>28.7</v>
       </c>
       <c r="M86" s="1">
-        <v>966012</v>
+        <v>276012</v>
       </c>
       <c r="N86" s="1">
-        <v>4788060</v>
+        <v>4104060</v>
       </c>
       <c r="O86">
         <v>287</v>
@@ -5546,16 +5546,16 @@
         <v>2700</v>
       </c>
       <c r="K87">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L87">
         <v>23.8</v>
       </c>
       <c r="M87" s="1">
-        <v>798012</v>
+        <v>228012</v>
       </c>
       <c r="N87" s="1">
-        <v>3948060</v>
+        <v>3384060</v>
       </c>
       <c r="O87">
         <v>237</v>
@@ -5602,16 +5602,16 @@
         <v>2754</v>
       </c>
       <c r="K88">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L88">
         <v>24.2</v>
       </c>
       <c r="M88" s="1">
-        <v>813970.799999999</v>
+        <v>232570.8</v>
       </c>
       <c r="N88" s="1">
-        <v>4032060</v>
+        <v>3456060</v>
       </c>
       <c r="O88">
         <v>242</v>
@@ -5658,16 +5658,16 @@
         <v>2835</v>
       </c>
       <c r="K89">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L89">
         <v>24.9</v>
       </c>
       <c r="M89" s="1">
-        <v>837912</v>
+        <v>239412</v>
       </c>
       <c r="N89" s="1">
-        <v>4116060</v>
+        <v>3528060</v>
       </c>
       <c r="O89">
         <v>249</v>
@@ -5714,16 +5714,16 @@
         <v>2943</v>
       </c>
       <c r="K90">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L90">
         <v>25.9</v>
       </c>
       <c r="M90" s="1">
-        <v>869832</v>
+        <v>248532</v>
       </c>
       <c r="N90" s="1">
-        <v>4284060</v>
+        <v>3672060</v>
       </c>
       <c r="O90">
         <v>258</v>
@@ -5770,16 +5770,16 @@
         <v>3104</v>
       </c>
       <c r="K91">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L91">
         <v>27.3</v>
       </c>
       <c r="M91" s="1">
-        <v>917712</v>
+        <v>262212</v>
       </c>
       <c r="N91" s="1">
-        <v>4536060</v>
+        <v>3888060</v>
       </c>
       <c r="O91">
         <v>273</v>
@@ -5835,7 +5835,7 @@
         <v>840012</v>
       </c>
       <c r="N92" s="1">
-        <v>5200060</v>
+        <v>4784060</v>
       </c>
       <c r="O92">
         <v>262</v>
@@ -5891,7 +5891,7 @@
         <v>856812</v>
       </c>
       <c r="N93" s="1">
-        <v>5300060</v>
+        <v>4876060</v>
       </c>
       <c r="O93">
         <v>267</v>
@@ -5947,7 +5947,7 @@
         <v>882012</v>
       </c>
       <c r="N94" s="1">
-        <v>5500060</v>
+        <v>5060060</v>
       </c>
       <c r="O94">
         <v>275</v>
@@ -6003,7 +6003,7 @@
         <v>915612</v>
       </c>
       <c r="N95" s="1">
-        <v>5700060</v>
+        <v>5244060</v>
       </c>
       <c r="O95">
         <v>286</v>
@@ -6059,7 +6059,7 @@
         <v>966012</v>
       </c>
       <c r="N96" s="1">
-        <v>6000060</v>
+        <v>5520060</v>
       </c>
       <c r="O96">
         <v>301</v>
@@ -6115,7 +6115,7 @@
         <v>800011.2</v>
       </c>
       <c r="N97" s="1">
-        <v>5000060</v>
+        <v>4600060</v>
       </c>
       <c r="O97">
         <v>250</v>
@@ -6171,7 +6171,7 @@
         <v>816012</v>
       </c>
       <c r="N98" s="1">
-        <v>5100060</v>
+        <v>4692060</v>
       </c>
       <c r="O98">
         <v>255</v>
@@ -6227,7 +6227,7 @@
         <v>840012</v>
       </c>
       <c r="N99" s="1">
-        <v>5200060</v>
+        <v>4784060</v>
       </c>
       <c r="O99">
         <v>262</v>
@@ -6283,7 +6283,7 @@
         <v>872011.2</v>
       </c>
       <c r="N100" s="1">
-        <v>5400060</v>
+        <v>4968060</v>
       </c>
       <c r="O100">
         <v>272</v>
@@ -6339,7 +6339,7 @@
         <v>920011.2</v>
       </c>
       <c r="N101" s="1">
-        <v>5700060</v>
+        <v>5244060</v>
       </c>
       <c r="O101">
         <v>287</v>
@@ -6395,7 +6395,7 @@
         <v>760011.6</v>
       </c>
       <c r="N102" s="1">
-        <v>4700060</v>
+        <v>4324060</v>
       </c>
       <c r="O102">
         <v>237</v>
@@ -6451,7 +6451,7 @@
         <v>775212</v>
       </c>
       <c r="N103" s="1">
-        <v>4800060</v>
+        <v>4416060</v>
       </c>
       <c r="O103">
         <v>242</v>
@@ -6507,7 +6507,7 @@
         <v>798012</v>
       </c>
       <c r="N104" s="1">
-        <v>4900060</v>
+        <v>4508060</v>
       </c>
       <c r="O104">
         <v>249</v>
@@ -6563,7 +6563,7 @@
         <v>828411.6</v>
       </c>
       <c r="N105" s="1">
-        <v>5100060</v>
+        <v>4692060</v>
       </c>
       <c r="O105">
         <v>258</v>
@@ -6619,7 +6619,7 @@
         <v>874011.6</v>
       </c>
       <c r="N106" s="1">
-        <v>5400060</v>
+        <v>4968060</v>
       </c>
       <c r="O106">
         <v>273</v>
@@ -6675,7 +6675,7 @@
         <v>420012</v>
       </c>
       <c r="N107" s="1">
-        <v>3952060</v>
+        <v>3744060</v>
       </c>
       <c r="O107">
         <v>262</v>
@@ -6731,7 +6731,7 @@
         <v>428412</v>
       </c>
       <c r="N108" s="1">
-        <v>4028060</v>
+        <v>3816060</v>
       </c>
       <c r="O108">
         <v>267</v>
@@ -6787,7 +6787,7 @@
         <v>441012</v>
       </c>
       <c r="N109" s="1">
-        <v>4180060</v>
+        <v>3960060</v>
       </c>
       <c r="O109">
         <v>275</v>
@@ -6843,7 +6843,7 @@
         <v>457812</v>
       </c>
       <c r="N110" s="1">
-        <v>4332060</v>
+        <v>4104060</v>
       </c>
       <c r="O110">
         <v>286</v>
@@ -6899,7 +6899,7 @@
         <v>483012</v>
       </c>
       <c r="N111" s="1">
-        <v>4560060</v>
+        <v>4320060</v>
       </c>
       <c r="O111">
         <v>301</v>
@@ -6955,7 +6955,7 @@
         <v>400011.6</v>
       </c>
       <c r="N112" s="1">
-        <v>3800060</v>
+        <v>3600060</v>
       </c>
       <c r="O112">
         <v>250</v>
@@ -7011,7 +7011,7 @@
         <v>408012</v>
       </c>
       <c r="N113" s="1">
-        <v>3876060</v>
+        <v>3672060</v>
       </c>
       <c r="O113">
         <v>255</v>
@@ -7067,7 +7067,7 @@
         <v>420012</v>
       </c>
       <c r="N114" s="1">
-        <v>3952060</v>
+        <v>3744060</v>
       </c>
       <c r="O114">
         <v>262</v>
@@ -7123,7 +7123,7 @@
         <v>436011.6</v>
       </c>
       <c r="N115" s="1">
-        <v>4104060</v>
+        <v>3888060</v>
       </c>
       <c r="O115">
         <v>272</v>
@@ -7179,7 +7179,7 @@
         <v>460011.6</v>
       </c>
       <c r="N116" s="1">
-        <v>4332060</v>
+        <v>4104060</v>
       </c>
       <c r="O116">
         <v>287</v>
@@ -7235,7 +7235,7 @@
         <v>380011.2</v>
       </c>
       <c r="N117" s="1">
-        <v>3572060</v>
+        <v>3384060</v>
       </c>
       <c r="O117">
         <v>237</v>
@@ -7291,7 +7291,7 @@
         <v>387612</v>
       </c>
       <c r="N118" s="1">
-        <v>3648060</v>
+        <v>3456060</v>
       </c>
       <c r="O118">
         <v>242</v>
@@ -7347,7 +7347,7 @@
         <v>399012</v>
       </c>
       <c r="N119" s="1">
-        <v>3724060</v>
+        <v>3528060</v>
       </c>
       <c r="O119">
         <v>249</v>
@@ -7403,7 +7403,7 @@
         <v>414211.2</v>
       </c>
       <c r="N120" s="1">
-        <v>3876060</v>
+        <v>3672060</v>
       </c>
       <c r="O120">
         <v>258</v>
@@ -7459,7 +7459,7 @@
         <v>437011.20000000001</v>
       </c>
       <c r="N121" s="1">
-        <v>4104060</v>
+        <v>3888060</v>
       </c>
       <c r="O121">
         <v>273</v>
@@ -7786,7 +7786,7 @@
         <v>1500</v>
       </c>
       <c r="K127">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L127">
         <v>28.3</v>
@@ -7842,7 +7842,7 @@
         <v>1530</v>
       </c>
       <c r="K128">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L128">
         <v>28.9</v>
@@ -7898,7 +7898,7 @@
         <v>1575</v>
       </c>
       <c r="K129">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L129">
         <v>29.8</v>
@@ -7954,7 +7954,7 @@
         <v>1635</v>
       </c>
       <c r="K130">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L130">
         <v>30</v>
@@ -8010,7 +8010,7 @@
         <v>1724</v>
       </c>
       <c r="K131">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L131">
         <v>30</v>
@@ -8066,7 +8066,7 @@
         <v>2700</v>
       </c>
       <c r="K132">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L132">
         <v>26.9</v>
@@ -8122,7 +8122,7 @@
         <v>2754</v>
       </c>
       <c r="K133">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L133">
         <v>27.5</v>
@@ -8178,7 +8178,7 @@
         <v>2835</v>
       </c>
       <c r="K134">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L134">
         <v>28.2</v>
@@ -8234,7 +8234,7 @@
         <v>2943</v>
       </c>
       <c r="K135">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L135">
         <v>29.3</v>
@@ -8290,7 +8290,7 @@
         <v>3104</v>
       </c>
       <c r="K136">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L136">
         <v>30</v>
@@ -8355,7 +8355,7 @@
         <v>1050015</v>
       </c>
       <c r="N137" s="1">
-        <v>3240060</v>
+        <v>3060060</v>
       </c>
       <c r="O137">
         <v>262</v>
@@ -8411,7 +8411,7 @@
         <v>1071015</v>
       </c>
       <c r="N138" s="1">
-        <v>3312060</v>
+        <v>3128060</v>
       </c>
       <c r="O138">
         <v>267</v>
@@ -8467,7 +8467,7 @@
         <v>1102515</v>
       </c>
       <c r="N139" s="1">
-        <v>3384060</v>
+        <v>3196060</v>
       </c>
       <c r="O139">
         <v>275</v>
@@ -8523,7 +8523,7 @@
         <v>1144515</v>
       </c>
       <c r="N140" s="1">
-        <v>3528060</v>
+        <v>3332060</v>
       </c>
       <c r="O140">
         <v>286</v>
@@ -8579,7 +8579,7 @@
         <v>1207515</v>
       </c>
       <c r="N141" s="1">
-        <v>3744060</v>
+        <v>3536060</v>
       </c>
       <c r="O141">
         <v>301</v>
@@ -8626,7 +8626,7 @@
         <v>1500</v>
       </c>
       <c r="K142">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L142">
         <v>28.3</v>
@@ -8635,7 +8635,7 @@
         <v>1000014</v>
       </c>
       <c r="N142" s="1">
-        <v>3096060</v>
+        <v>2924060</v>
       </c>
       <c r="O142">
         <v>250</v>
@@ -8682,7 +8682,7 @@
         <v>1530</v>
       </c>
       <c r="K143">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L143">
         <v>28.9</v>
@@ -8691,7 +8691,7 @@
         <v>1020015</v>
       </c>
       <c r="N143" s="1">
-        <v>3168060</v>
+        <v>2992060</v>
       </c>
       <c r="O143">
         <v>255</v>
@@ -8738,7 +8738,7 @@
         <v>1575</v>
       </c>
       <c r="K144">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L144">
         <v>29.8</v>
@@ -8747,7 +8747,7 @@
         <v>1050015</v>
       </c>
       <c r="N144" s="1">
-        <v>3240060</v>
+        <v>3060060</v>
       </c>
       <c r="O144">
         <v>262</v>
@@ -8794,7 +8794,7 @@
         <v>1635</v>
       </c>
       <c r="K145">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L145">
         <v>30</v>
@@ -8803,7 +8803,7 @@
         <v>1090014</v>
       </c>
       <c r="N145" s="1">
-        <v>3384060</v>
+        <v>3196060</v>
       </c>
       <c r="O145">
         <v>272</v>
@@ -8850,7 +8850,7 @@
         <v>1724</v>
       </c>
       <c r="K146">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L146">
         <v>30</v>
@@ -8859,7 +8859,7 @@
         <v>1150014</v>
       </c>
       <c r="N146" s="1">
-        <v>3528060</v>
+        <v>3332060</v>
       </c>
       <c r="O146">
         <v>287</v>
@@ -8906,7 +8906,7 @@
         <v>2700</v>
       </c>
       <c r="K147">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L147">
         <v>26.9</v>
@@ -8915,7 +8915,7 @@
         <v>950014.5</v>
       </c>
       <c r="N147" s="1">
-        <v>2952060</v>
+        <v>2788060</v>
       </c>
       <c r="O147">
         <v>237</v>
@@ -8962,7 +8962,7 @@
         <v>2754</v>
       </c>
       <c r="K148">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L148">
         <v>27.5</v>
@@ -8971,7 +8971,7 @@
         <v>969015</v>
       </c>
       <c r="N148" s="1">
-        <v>2952060</v>
+        <v>2788060</v>
       </c>
       <c r="O148">
         <v>242</v>
@@ -9018,7 +9018,7 @@
         <v>2835</v>
       </c>
       <c r="K149">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L149">
         <v>28.2</v>
@@ -9027,7 +9027,7 @@
         <v>997515</v>
       </c>
       <c r="N149" s="1">
-        <v>3096060</v>
+        <v>2924060</v>
       </c>
       <c r="O149">
         <v>249</v>
@@ -9074,7 +9074,7 @@
         <v>2943</v>
       </c>
       <c r="K150">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L150">
         <v>29.3</v>
@@ -9083,7 +9083,7 @@
         <v>1035514.5</v>
       </c>
       <c r="N150" s="1">
-        <v>3168060</v>
+        <v>2992060</v>
       </c>
       <c r="O150">
         <v>258</v>
@@ -9130,7 +9130,7 @@
         <v>3104</v>
       </c>
       <c r="K151">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L151">
         <v>30</v>
@@ -9139,7 +9139,7 @@
         <v>1092514.5</v>
       </c>
       <c r="N151" s="1">
-        <v>3384060</v>
+        <v>3196060</v>
       </c>
       <c r="O151">
         <v>273</v>
@@ -9466,7 +9466,7 @@
         <v>1500</v>
       </c>
       <c r="K157">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L157">
         <v>28.3</v>
@@ -9522,7 +9522,7 @@
         <v>1530</v>
       </c>
       <c r="K158">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L158">
         <v>28.9</v>
@@ -9578,7 +9578,7 @@
         <v>1575</v>
       </c>
       <c r="K159">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L159">
         <v>29.8</v>
@@ -9634,7 +9634,7 @@
         <v>1635</v>
       </c>
       <c r="K160">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L160">
         <v>30</v>
@@ -9690,7 +9690,7 @@
         <v>1724</v>
       </c>
       <c r="K161">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L161">
         <v>30</v>
@@ -9746,7 +9746,7 @@
         <v>2700</v>
       </c>
       <c r="K162">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L162">
         <v>26.9</v>
@@ -9802,7 +9802,7 @@
         <v>2754</v>
       </c>
       <c r="K163">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L163">
         <v>27.5</v>
@@ -9858,7 +9858,7 @@
         <v>2835</v>
       </c>
       <c r="K164">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L164">
         <v>28.2</v>
@@ -9914,7 +9914,7 @@
         <v>2943</v>
       </c>
       <c r="K165">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L165">
         <v>29.3</v>
@@ -9970,7 +9970,7 @@
         <v>3104</v>
       </c>
       <c r="K166">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L166">
         <v>30</v>
@@ -10306,7 +10306,7 @@
         <v>1500</v>
       </c>
       <c r="K172">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L172">
         <v>28.3</v>
@@ -10362,7 +10362,7 @@
         <v>1530</v>
       </c>
       <c r="K173">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L173">
         <v>28.9</v>
@@ -10418,7 +10418,7 @@
         <v>1575</v>
       </c>
       <c r="K174">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L174">
         <v>29.8</v>
@@ -10474,7 +10474,7 @@
         <v>1635</v>
       </c>
       <c r="K175">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L175">
         <v>30</v>
@@ -10530,7 +10530,7 @@
         <v>1724</v>
       </c>
       <c r="K176">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L176">
         <v>30</v>
@@ -10586,7 +10586,7 @@
         <v>2700</v>
       </c>
       <c r="K177">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L177">
         <v>26.9</v>
@@ -10642,7 +10642,7 @@
         <v>2754</v>
       </c>
       <c r="K178">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L178">
         <v>27.5</v>
@@ -10698,7 +10698,7 @@
         <v>2835</v>
       </c>
       <c r="K179">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L179">
         <v>28.2</v>
@@ -10754,7 +10754,7 @@
         <v>2943</v>
       </c>
       <c r="K180">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L180">
         <v>29.3</v>
@@ -10810,7 +10810,7 @@
         <v>3104</v>
       </c>
       <c r="K181">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L181">
         <v>30</v>

</xml_diff>